<commit_message>
Pending: Report and Highlighter
</commit_message>
<xml_diff>
--- a/identifyCourse/Input/Input.xlsx
+++ b/identifyCourse/Input/Input.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\922137\git\Hackathon\identifyCourse\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDF85A7-DF61-4AC2-AAF6-0CEDC2FD1BFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" tabRatio="500"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="26">
   <si>
     <t>Country</t>
   </si>
@@ -38,18 +39,12 @@
     <t>ABC</t>
   </si>
   <si>
-    <t>abc123@gma</t>
-  </si>
-  <si>
     <t>123-456-7890</t>
   </si>
   <si>
     <t>mvn institute</t>
   </si>
   <si>
-    <t>www.mvn.com</t>
-  </si>
-  <si>
     <t>India</t>
   </si>
   <si>
@@ -59,12 +54,6 @@
     <t xml:space="preserve">    </t>
   </si>
   <si>
-    <t xml:space="preserve">     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">      </t>
-  </si>
-  <si>
     <t>abc123@gmail.com</t>
   </si>
   <si>
@@ -86,17 +75,41 @@
     <t>Inst._Name</t>
   </si>
   <si>
-    <t>Inst._Url</t>
-  </si>
-  <si>
-    <t>No._ Of_Learners</t>
+    <t>Job Function</t>
+  </si>
+  <si>
+    <t>Dean</t>
+  </si>
+  <si>
+    <t>Institution Type</t>
+  </si>
+  <si>
+    <t>Government</t>
+  </si>
+  <si>
+    <t>Discipline</t>
+  </si>
+  <si>
+    <t>Architecture</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Tamil Nadu</t>
+  </si>
+  <si>
+    <t>123-456-7891</t>
+  </si>
+  <si>
+    <t>123-456-7892</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -117,6 +130,12 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -424,170 +443,191 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" customWidth="1"/>
-    <col min="5" max="5" width="25.88671875" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" customWidth="1"/>
+    <col min="4" max="4" width="13.90625" customWidth="1"/>
+    <col min="5" max="5" width="20.08984375" customWidth="1"/>
+    <col min="6" max="6" width="25.90625" customWidth="1"/>
+    <col min="7" max="7" width="12.6328125" customWidth="1"/>
+    <col min="8" max="8" width="20.08984375" customWidth="1"/>
+    <col min="9" max="9" width="16.36328125" customWidth="1"/>
+    <col min="11" max="11" width="11.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
         <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
       <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2">
-        <v>40</v>
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
       <c r="G3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3">
-        <v>40</v>
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
       </c>
       <c r="I3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4">
-        <v>40</v>
-      </c>
-      <c r="I4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>5</v>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5">
-        <v>40</v>
+        <v>5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>19</v>
       </c>
       <c r="I5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="J5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -595,28 +635,34 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s">
-        <v>5</v>
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6">
-        <v>40</v>
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>19</v>
       </c>
       <c r="I6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="J6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -624,28 +670,34 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" t="s">
-        <v>5</v>
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7">
-        <v>40</v>
+        <v>5</v>
+      </c>
+      <c r="H7" t="s">
+        <v>19</v>
       </c>
       <c r="I7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="J7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -653,28 +705,34 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" t="s">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8">
-        <v>40</v>
+        <v>5</v>
+      </c>
+      <c r="H8" t="s">
+        <v>19</v>
       </c>
       <c r="I8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="J8" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -682,28 +740,34 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" t="s">
-        <v>5</v>
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G9" t="s">
         <v>7</v>
       </c>
-      <c r="H9">
-        <v>40</v>
+      <c r="H9" t="s">
+        <v>19</v>
       </c>
       <c r="I9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="J9" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -711,28 +775,31 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" t="s">
-        <v>5</v>
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="I10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="J10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -740,72 +807,107 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" t="s">
-        <v>5</v>
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="J11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G12" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H12" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="I12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D13" s="1"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="D5" r:id="rId4"/>
-    <hyperlink ref="D6" r:id="rId5"/>
-    <hyperlink ref="D8" r:id="rId6"/>
-    <hyperlink ref="D9" r:id="rId7"/>
-    <hyperlink ref="D10" r:id="rId8"/>
-    <hyperlink ref="D11" r:id="rId9"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E12" r:id="rId9" xr:uid="{07A83A0F-6035-4BDB-AD11-656E554BECB4}"/>
+    <hyperlink ref="E13" r:id="rId10" xr:uid="{85B3EEC4-0D50-4A58-BB6D-DA9E1FA41F7A}"/>
+    <hyperlink ref="E3" r:id="rId11" xr:uid="{E4AD86BC-9A4E-4773-987C-08C1E96F6090}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId10"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>